<commit_message>
added abstract, minutes and requirements
</commit_message>
<xml_diff>
--- a/trunk/Documentation/ProjectDocumentation/Time_recording.xlsx
+++ b/trunk/Documentation/ProjectDocumentation/Time_recording.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bliznac\Desktop\Git-Repository_Project\aerojump\trunk\Documentation\ProjectDocumentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7425" yWindow="-15" windowWidth="7485" windowHeight="10590" activeTab="2"/>
+    <workbookView xWindow="7425" yWindow="-15" windowWidth="7485" windowHeight="10590" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="7" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1649" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="130">
   <si>
     <t>Nr</t>
   </si>
@@ -390,6 +390,36 @@
   </si>
   <si>
     <t>InfoActivity (How To Play) implementiert</t>
+  </si>
+  <si>
+    <t>Brainstorming,Implementation, Documentation</t>
+  </si>
+  <si>
+    <t>Implementation, Documentation</t>
+  </si>
+  <si>
+    <t>Implementation</t>
+  </si>
+  <si>
+    <t>Individual Work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presentation </t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Brainstorming, looking for ideas</t>
+  </si>
+  <si>
+    <t>Brainstorming, searching web for ideas</t>
+  </si>
+  <si>
+    <t>Brainstorming, forming the actual idea</t>
+  </si>
+  <si>
+    <t>Implementation, Documentation, Design</t>
   </si>
 </sst>
 </file>
@@ -2125,7 +2155,7 @@
   </sheetPr>
   <dimension ref="B2:AG55"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="F8" workbookViewId="0">
       <selection activeCell="E2" sqref="E2:I2"/>
     </sheetView>
   </sheetViews>
@@ -3182,11 +3212,11 @@
       </c>
       <c r="F19" s="146">
         <f t="shared" ref="F19" si="9">IF(NOT(EXACT($B19,"----")),SUM($J20,IF($E$3&gt;=2,$K20,0),IF($E$3&gt;=3,$L20,0),IF($E$3&gt;=4,$M20,0),IF($E$3&gt;=5,$N20,0),IF($E$3&gt;=6,$O20,0),IF($E$3&gt;=7,$P20,0),IF($E$3&gt;=8,$Q20,0),IF($E$3&gt;=9,$R20,0),IF($E$3&gt;=10,$S20,0),IF($E$3&gt;=11,$T20,0),IF($E$3&gt;=12,$U20,0),IF($E$3&gt;=13,$V20,0),IF($E$3&gt;=14,$W20,0),IF($E$3&gt;=15,$X20,0),IF($E$3&gt;=16,$Y20,0),IF($E$3&gt;=17,$Z20,0),IF($E$3&gt;=18,$AA20,0),IF($E$3&gt;=19,$AB20,0),IF($E$3&gt;=20,$AC20,0)),0)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G19" s="102">
         <f t="shared" ref="G19" si="10">F19-E19</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H19" s="157"/>
       <c r="I19" s="41" t="s">
@@ -3282,7 +3312,7 @@
       </c>
       <c r="AF19" s="160">
         <f>AD20-AE19</f>
-        <v>-69</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="2:32" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3298,35 +3328,35 @@
       </c>
       <c r="J20" s="32">
         <f>'Std-C'!C12</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K20" s="32">
         <f>'Std-C'!C23</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L20" s="32">
         <f>'Std-C'!C34</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M20" s="32">
         <f>'Std-C'!C45</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="N20" s="32">
         <f>'Std-C'!C56</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="O20" s="32">
         <f>'Std-C'!C67</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="P20" s="32">
         <f>'Std-C'!C78</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="Q20" s="32">
         <f>'Std-C'!C89</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="R20" s="32">
         <f>'Std-C'!C100</f>
@@ -3378,7 +3408,7 @@
       </c>
       <c r="AD20" s="33">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>77</v>
       </c>
       <c r="AE20" s="68"/>
       <c r="AF20" s="81"/>
@@ -3396,35 +3426,35 @@
       </c>
       <c r="J21" s="29">
         <f t="shared" ref="J21:U21" si="11">J20-J19</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K21" s="29">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L21" s="29">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M21" s="29">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="N21" s="29">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="O21" s="29">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="P21" s="29">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="Q21" s="29">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="R21" s="29">
         <f t="shared" si="11"/>
@@ -3476,7 +3506,7 @@
       </c>
       <c r="AD21" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="AE21" s="69"/>
       <c r="AF21" s="82"/>
@@ -4752,7 +4782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E223"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17:C17"/>
     </sheetView>
   </sheetViews>
@@ -7493,7 +7523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -10276,8 +10306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E223"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A231" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10363,12 +10393,18 @@
       <c r="A7" s="46">
         <v>2</v>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="43"/>
+      <c r="B7" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="43">
+        <v>180</v>
+      </c>
       <c r="D7" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="42"/>
+      <c r="E7" s="42" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="8" spans="1:5" s="47" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="46">
@@ -10421,7 +10457,7 @@
       <c r="B12" s="173"/>
       <c r="C12" s="25">
         <f>ROUND((SUM(C6:C11)/60),0)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D12" s="162" t="s">
         <v>18</v>
@@ -10489,19 +10525,25 @@
         <v>17</v>
       </c>
       <c r="E17" s="42" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="47" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="46">
         <v>2</v>
       </c>
-      <c r="B18" s="42"/>
-      <c r="C18" s="43"/>
+      <c r="B18" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="C18" s="43">
+        <v>180</v>
+      </c>
       <c r="D18" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="42"/>
+      <c r="E18" s="42" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="19" spans="1:5" s="47" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="46">
@@ -10554,7 +10596,7 @@
       <c r="B23" s="163"/>
       <c r="C23" s="25">
         <f>ROUND((SUM(C17:C22)/60),0)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D23" s="162" t="s">
         <v>18</v>
@@ -10612,23 +10654,35 @@
       <c r="A28" s="46">
         <v>1</v>
       </c>
-      <c r="B28" s="42"/>
-      <c r="C28" s="43"/>
+      <c r="B28" s="47" t="s">
+        <v>123</v>
+      </c>
+      <c r="C28" s="47">
+        <v>120</v>
+      </c>
       <c r="D28" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="E28" s="42"/>
+      <c r="E28" s="47" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="29" spans="1:5" s="47" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="46">
         <v>2</v>
       </c>
-      <c r="B29" s="42"/>
-      <c r="C29" s="43"/>
+      <c r="B29" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="C29" s="43">
+        <v>180</v>
+      </c>
       <c r="D29" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="E29" s="42"/>
+      <c r="E29" s="42" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="30" spans="1:5" s="47" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="46">
@@ -10681,7 +10735,7 @@
       <c r="B34" s="163"/>
       <c r="C34" s="25">
         <f>ROUND((SUM(C28:C33)/60),0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D34" s="162" t="s">
         <v>18</v>
@@ -10739,23 +10793,35 @@
       <c r="A39" s="46">
         <v>1</v>
       </c>
-      <c r="B39" s="42"/>
-      <c r="C39" s="43"/>
+      <c r="B39" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39" s="43">
+        <v>150</v>
+      </c>
       <c r="D39" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="E39" s="42"/>
+      <c r="E39" s="42" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="40" spans="1:5" s="47" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="46">
         <v>2</v>
       </c>
-      <c r="B40" s="42"/>
-      <c r="C40" s="43"/>
+      <c r="B40" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" s="43">
+        <v>360</v>
+      </c>
       <c r="D40" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="E40" s="42"/>
+      <c r="E40" s="42" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="41" spans="1:5" s="47" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="46">
@@ -10808,7 +10874,7 @@
       <c r="B45" s="163"/>
       <c r="C45" s="25">
         <f>ROUND((SUM(C39:C44)/60),0)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D45" s="162" t="s">
         <v>18</v>
@@ -10866,23 +10932,35 @@
       <c r="A50" s="46">
         <v>1</v>
       </c>
-      <c r="B50" s="42"/>
-      <c r="C50" s="43"/>
+      <c r="B50" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="C50" s="43">
+        <v>240</v>
+      </c>
       <c r="D50" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="E50" s="42"/>
+      <c r="E50" s="42" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="51" spans="1:5" s="47" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="46">
         <v>2</v>
       </c>
-      <c r="B51" s="42"/>
-      <c r="C51" s="43"/>
+      <c r="B51" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="C51" s="43">
+        <v>180</v>
+      </c>
       <c r="D51" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="E51" s="42"/>
+      <c r="E51" s="42" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="52" spans="1:5" s="47" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="46">
@@ -10935,7 +11013,7 @@
       <c r="B56" s="163"/>
       <c r="C56" s="25">
         <f>ROUND((SUM(C50:C55)/60),0)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D56" s="162" t="s">
         <v>18</v>
@@ -10993,34 +11071,52 @@
       <c r="A61" s="46">
         <v>1</v>
       </c>
-      <c r="B61" s="42"/>
-      <c r="C61" s="43"/>
+      <c r="B61" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="C61" s="43">
+        <v>240</v>
+      </c>
       <c r="D61" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="E61" s="42"/>
+      <c r="E61" s="42" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="62" spans="1:5" s="47" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="46">
         <v>2</v>
       </c>
-      <c r="B62" s="42"/>
-      <c r="C62" s="43"/>
+      <c r="B62" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="C62" s="43">
+        <v>480</v>
+      </c>
       <c r="D62" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="E62" s="42"/>
+      <c r="E62" s="42" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="63" spans="1:5" s="47" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="46">
         <v>3</v>
       </c>
-      <c r="B63" s="42"/>
-      <c r="C63" s="43"/>
+      <c r="B63" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="C63" s="43">
+        <v>120</v>
+      </c>
       <c r="D63" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="E63" s="42"/>
+      <c r="E63" s="42" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="64" spans="1:5" s="47" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="46">
@@ -11062,7 +11158,7 @@
       <c r="B67" s="163"/>
       <c r="C67" s="25">
         <f>ROUND((SUM(C61:C66)/60),0)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D67" s="162" t="s">
         <v>18</v>
@@ -11120,34 +11216,52 @@
       <c r="A72" s="46">
         <v>1</v>
       </c>
-      <c r="B72" s="42"/>
-      <c r="C72" s="43"/>
+      <c r="B72" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="C72" s="43">
+        <v>420</v>
+      </c>
       <c r="D72" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="E72" s="42"/>
+      <c r="E72" s="42" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="73" spans="1:5" s="47" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="46">
         <v>2</v>
       </c>
-      <c r="B73" s="42"/>
-      <c r="C73" s="43"/>
+      <c r="B73" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="C73" s="43">
+        <v>120</v>
+      </c>
       <c r="D73" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="E73" s="42"/>
+      <c r="E73" s="42" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="74" spans="1:5" s="47" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="46">
         <v>3</v>
       </c>
-      <c r="B74" s="42"/>
-      <c r="C74" s="43"/>
+      <c r="B74" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="C74" s="43">
+        <v>360</v>
+      </c>
       <c r="D74" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="E74" s="42"/>
+      <c r="E74" s="42" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="75" spans="1:5" s="47" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="46">
@@ -11189,7 +11303,7 @@
       <c r="B78" s="163"/>
       <c r="C78" s="25">
         <f>ROUND((SUM(C72:C77)/60),0)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D78" s="162" t="s">
         <v>18</v>
@@ -11247,34 +11361,52 @@
       <c r="A83" s="46">
         <v>1</v>
       </c>
-      <c r="B83" s="42"/>
-      <c r="C83" s="43"/>
+      <c r="B83" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="C83" s="43">
+        <v>480</v>
+      </c>
       <c r="D83" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="E83" s="42"/>
+      <c r="E83" s="42" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="84" spans="1:5" s="47" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="46">
         <v>2</v>
       </c>
-      <c r="B84" s="42"/>
-      <c r="C84" s="43"/>
+      <c r="B84" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="C84" s="43">
+        <v>240</v>
+      </c>
       <c r="D84" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="E84" s="42"/>
+      <c r="E84" s="42" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="85" spans="1:5" s="47" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="46">
         <v>3</v>
       </c>
-      <c r="B85" s="42"/>
-      <c r="C85" s="43"/>
+      <c r="B85" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="C85" s="43">
+        <v>160</v>
+      </c>
       <c r="D85" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="E85" s="42"/>
+      <c r="E85" s="42" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="86" spans="1:5" s="47" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="46">
@@ -11316,7 +11448,7 @@
       <c r="B89" s="163"/>
       <c r="C89" s="25">
         <f>ROUND((SUM(C83:C88)/60),0)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D89" s="162" t="s">
         <v>18</v>

</xml_diff>